<commit_message>
alter catia data and epochs
</commit_message>
<xml_diff>
--- a/src/core/catia_data.xlsx
+++ b/src/core/catia_data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29401"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A94F17C-F2D9-419B-8EA1-F3364FB0225A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BBB9AF4-AF97-4BE3-9DAD-F20612432681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>X(mm)</t>
+    <t>x</t>
   </si>
   <si>
-    <t>Value(N_m2)</t>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -72,9 +72,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,11 +408,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -425,114 +429,954 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.32915299999999997</v>
-      </c>
-      <c r="B2" s="1">
-        <v>76964000</v>
+        <v>0.25</v>
+      </c>
+      <c r="B2">
+        <v>3.5963099999999995E-5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>4.5119999999999996</v>
-      </c>
-      <c r="B3" s="1">
-        <v>96579800</v>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="B3">
+        <v>3.5617899999999998E-4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>10.0891</v>
-      </c>
-      <c r="B4" s="1">
-        <v>63551600</v>
+        <v>1.024</v>
+      </c>
+      <c r="B4">
+        <v>3.4425699999999999E-4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>13.536</v>
-      </c>
-      <c r="B5" s="1">
-        <v>80521000</v>
+        <v>1.536</v>
+      </c>
+      <c r="B5">
+        <v>3.5540399999999997E-4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>19.113099999999999</v>
-      </c>
-      <c r="B6" s="1">
-        <v>47362700</v>
+        <v>2.048</v>
+      </c>
+      <c r="B6">
+        <v>3.4369799999999997E-4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>23.092600000000001</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45979500</v>
+        <v>2.56</v>
+      </c>
+      <c r="B7">
+        <v>3.5581299999999996E-4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>27.071999999999999</v>
-      </c>
-      <c r="B8" s="1">
-        <v>43644200</v>
+        <v>3.10663</v>
+      </c>
+      <c r="B8">
+        <v>3.4347299999999996E-4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>31.584</v>
-      </c>
-      <c r="B9" s="1">
-        <v>38704300</v>
+        <v>3.5466500000000001</v>
+      </c>
+      <c r="B9">
+        <v>3.53839E-4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>36.095999999999997</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45832400</v>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="B10">
+        <v>3.3994899999999998E-4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>41.140599999999999</v>
-      </c>
-      <c r="B11" s="1">
-        <v>22871400</v>
+        <v>4.6079999999999997</v>
+      </c>
+      <c r="B11">
+        <v>3.50603E-4</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>45.12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>25530700</v>
+        <v>5.12</v>
+      </c>
+      <c r="B12">
+        <v>3.3592099999999998E-4</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>49.302799999999998</v>
-      </c>
-      <c r="B13" s="1">
-        <v>21047000</v>
+        <v>5.6319999999999997</v>
+      </c>
+      <c r="B13">
+        <v>3.4440399999999998E-4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>54.143999999999998</v>
-      </c>
-      <c r="B14" s="1">
-        <v>16383600</v>
+        <v>6.1440000000000001</v>
+      </c>
+      <c r="B14">
+        <v>3.2943499999999999E-4</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
+        <v>6.6559999999999997</v>
+      </c>
+      <c r="B15">
+        <v>3.3709699999999996E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>7.1680000000000001</v>
+      </c>
+      <c r="B16">
+        <v>3.21358E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>7.68</v>
+      </c>
+      <c r="B17">
+        <v>3.2782899999999997E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>8.2524300000000004</v>
+      </c>
+      <c r="B18">
+        <v>3.1239799999999997E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>8.7040000000000006</v>
+      </c>
+      <c r="B19">
+        <v>3.18762E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>9.1786499999999993</v>
+      </c>
+      <c r="B20">
+        <v>3.0251799999999999E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>9.7279999999999998</v>
+      </c>
+      <c r="B21">
+        <v>3.0687099999999996E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>10.24</v>
+      </c>
+      <c r="B22">
+        <v>2.9076699999999999E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>10.752000000000001</v>
+      </c>
+      <c r="B23">
+        <v>2.9489399999999997E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>11.301399999999999</v>
+      </c>
+      <c r="B24">
+        <v>2.7930499999999998E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>11.776</v>
+      </c>
+      <c r="B25">
+        <v>2.8345599999999996E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>12.2506</v>
+      </c>
+      <c r="B26">
+        <v>2.6824299999999999E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>12.8</v>
+      </c>
+      <c r="B27">
+        <v>2.71721E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>13.311999999999999</v>
+      </c>
+      <c r="B28">
+        <v>2.5705599999999997E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>13.824</v>
+      </c>
+      <c r="B29">
+        <v>2.60256E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>14.336</v>
+      </c>
+      <c r="B30">
+        <v>2.4545399999999998E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>14.848000000000001</v>
+      </c>
+      <c r="B31">
+        <v>2.48237E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>15.394600000000001</v>
+      </c>
+      <c r="B32">
+        <v>2.3474999999999999E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>15.8347</v>
+      </c>
+      <c r="B33">
+        <v>2.3701499999999998E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>16.418600000000001</v>
+      </c>
+      <c r="B34">
+        <v>2.23723E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>16.858699999999999</v>
+      </c>
+      <c r="B35">
+        <v>2.27388E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>17.408000000000001</v>
+      </c>
+      <c r="B36">
+        <v>2.1389699999999997E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>17.8827</v>
+      </c>
+      <c r="B37">
+        <v>2.1635599999999999E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>18.431999999999999</v>
+      </c>
+      <c r="B38">
+        <v>2.0325199999999998E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>18.943999999999999</v>
+      </c>
+      <c r="B39">
+        <v>2.05706E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>19.418600000000001</v>
+      </c>
+      <c r="B40">
+        <v>1.9356999999999998E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>19.968</v>
+      </c>
+      <c r="B41">
+        <v>1.9553299999999999E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>20.517399999999999</v>
+      </c>
+      <c r="B42">
+        <v>1.8433799999999998E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>20.992000000000001</v>
+      </c>
+      <c r="B43">
+        <v>1.86472E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>21.504000000000001</v>
+      </c>
+      <c r="B44">
+        <v>1.7547199999999998E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>22.015999999999998</v>
+      </c>
+      <c r="B45">
+        <v>1.7712899999999999E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>22.527999999999999</v>
+      </c>
+      <c r="B46">
+        <v>1.6610599999999998E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>23.04</v>
+      </c>
+      <c r="B47">
+        <v>1.67548E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>23.552</v>
+      </c>
+      <c r="B48">
+        <v>1.5709099999999999E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>24.064</v>
+      </c>
+      <c r="B49">
+        <v>1.5857599999999998E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>24.576000000000001</v>
+      </c>
+      <c r="B50">
+        <v>1.48546E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>25.088000000000001</v>
+      </c>
+      <c r="B51">
+        <v>1.4985499999999998E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>25.6</v>
+      </c>
+      <c r="B52">
+        <v>1.4048999999999998E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>26.111999999999998</v>
+      </c>
+      <c r="B53">
+        <v>1.4141799999999998E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>26.68</v>
+      </c>
+      <c r="B54">
+        <v>1.3246899999999999E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>27.098700000000001</v>
+      </c>
+      <c r="B55">
+        <v>1.34182E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>27.648</v>
+      </c>
+      <c r="B56">
+        <v>1.24981E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>28.16</v>
+      </c>
+      <c r="B57">
+        <v>1.25711E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>28.672000000000001</v>
+      </c>
+      <c r="B58">
+        <v>1.17129E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>29.184000000000001</v>
+      </c>
+      <c r="B59">
+        <v>1.1770599999999999E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>29.7334</v>
+      </c>
+      <c r="B60">
+        <v>1.09831E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>30.238199999999999</v>
+      </c>
+      <c r="B61">
+        <v>1.1107099999999999E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>30.622199999999999</v>
+      </c>
+      <c r="B62">
+        <v>1.0462E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>31.088100000000001</v>
+      </c>
+      <c r="B63">
+        <v>1.01536E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>31.781400000000001</v>
+      </c>
+      <c r="B64">
+        <v>9.5700799999999997E-5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>32.256</v>
+      </c>
+      <c r="B65">
+        <v>9.6945699999999996E-5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>32.768000000000001</v>
+      </c>
+      <c r="B66">
+        <v>8.9526899999999992E-5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>33.28</v>
+      </c>
+      <c r="B67">
+        <v>8.9954E-5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>33.8294</v>
+      </c>
+      <c r="B68">
+        <v>8.2939299999999994E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>34.304000000000002</v>
+      </c>
+      <c r="B69">
+        <v>8.3670499999999998E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>34.853400000000001</v>
+      </c>
+      <c r="B70">
+        <v>7.7093000000000002E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>35.328000000000003</v>
+      </c>
+      <c r="B71">
+        <v>7.7558099999999999E-5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>35.877400000000002</v>
+      </c>
+      <c r="B72">
+        <v>7.1441599999999997E-5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>36.351999999999997</v>
+      </c>
+      <c r="B73">
+        <v>7.2386100000000001E-5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>36.863999999999997</v>
+      </c>
+      <c r="B74">
+        <v>6.6137599999999995E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>37.413400000000003</v>
+      </c>
+      <c r="B75">
+        <v>6.7234699999999995E-5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>37.832000000000001</v>
+      </c>
+      <c r="B76">
+        <v>6.0858899999999994E-5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <v>38.4</v>
+      </c>
+      <c r="B77">
+        <v>6.11336E-5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <v>38.874699999999997</v>
+      </c>
+      <c r="B78">
+        <v>5.5519599999999996E-5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <v>39.423999999999999</v>
+      </c>
+      <c r="B79">
+        <v>5.5936099999999995E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <v>39.936</v>
+      </c>
+      <c r="B80">
+        <v>5.0516099999999996E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <v>40.448</v>
+      </c>
+      <c r="B81">
+        <v>5.1030399999999998E-5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82">
+        <v>41.020400000000002</v>
+      </c>
+      <c r="B82">
+        <v>4.6202299999999996E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83">
+        <v>41.472000000000001</v>
+      </c>
+      <c r="B83">
+        <v>4.7635999999999996E-5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84">
+        <v>41.984000000000002</v>
+      </c>
+      <c r="B84">
+        <v>4.19205E-5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85">
+        <v>42.496000000000002</v>
+      </c>
+      <c r="B85">
+        <v>4.2819599999999999E-5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86">
+        <v>43.008000000000003</v>
+      </c>
+      <c r="B86">
+        <v>3.7580699999999997E-5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87">
+        <v>43.52</v>
+      </c>
+      <c r="B87">
+        <v>3.82771E-5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88">
+        <v>44.031999999999996</v>
+      </c>
+      <c r="B88">
+        <v>3.3691799999999995E-5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89">
+        <v>44.543999999999997</v>
+      </c>
+      <c r="B89">
+        <v>3.4388499999999998E-5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90">
+        <v>45.093400000000003</v>
+      </c>
+      <c r="B90">
+        <v>3.0127999999999997E-5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91">
+        <v>45.567999999999998</v>
+      </c>
+      <c r="B91">
+        <v>3.1169600000000001E-5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92">
+        <v>46.1404</v>
+      </c>
+      <c r="B92">
+        <v>2.6999099999999997E-5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93">
+        <v>46.629399999999997</v>
+      </c>
+      <c r="B93">
+        <v>2.91651E-5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94">
+        <v>47.103999999999999</v>
+      </c>
+      <c r="B94">
+        <v>2.4154799999999998E-5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95">
+        <v>47.616</v>
+      </c>
+      <c r="B95">
+        <v>2.5398999999999999E-5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96">
+        <v>48.165399999999998</v>
+      </c>
+      <c r="B96">
+        <v>2.1410199999999997E-5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97">
+        <v>48.64</v>
+      </c>
+      <c r="B97">
+        <v>2.3671199999999998E-5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98">
+        <v>49.152000000000001</v>
+      </c>
+      <c r="B98">
+        <v>1.8879E-5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99">
+        <v>49.664000000000001</v>
+      </c>
+      <c r="B99">
+        <v>2.1033699999999998E-5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100">
+        <v>50.176000000000002</v>
+      </c>
+      <c r="B100">
+        <v>1.6564600000000001E-5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101">
+        <v>50.688000000000002</v>
+      </c>
+      <c r="B101">
+        <v>1.8751799999999999E-5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102">
+        <v>51.2</v>
+      </c>
+      <c r="B102">
+        <v>1.4586899999999999E-5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103">
+        <v>51.712000000000003</v>
+      </c>
+      <c r="B103">
+        <v>1.72905E-5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104">
+        <v>52.223999999999997</v>
+      </c>
+      <c r="B104">
+        <v>1.2992199999999999E-5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105">
+        <v>52.735999999999997</v>
+      </c>
+      <c r="B105">
+        <v>1.5892899999999998E-5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106">
+        <v>53.247999999999998</v>
+      </c>
+      <c r="B106">
+        <v>1.1693299999999999E-5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107">
+        <v>53.76</v>
+      </c>
+      <c r="B107">
+        <v>1.5060899999999998E-5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108">
+        <v>54.271999999999998</v>
+      </c>
+      <c r="B108">
+        <v>1.06655E-5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109">
+        <v>54.783999999999999</v>
+      </c>
+      <c r="B109">
+        <v>1.3932199999999999E-5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110">
+        <v>55.295999999999999</v>
+      </c>
+      <c r="B110">
+        <v>9.8735699999999994E-6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111">
+        <v>55.808</v>
+      </c>
+      <c r="B111">
+        <v>1.38524E-5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112">
+        <v>56.32</v>
+      </c>
+      <c r="B112">
+        <v>9.3269099999999994E-6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113">
+        <v>56.832000000000001</v>
+      </c>
+      <c r="B113">
+        <v>1.33233E-5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114">
+        <v>57.344000000000001</v>
+      </c>
+      <c r="B114">
+        <v>9.0454699999999996E-6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115">
+        <v>57.856000000000002</v>
+      </c>
+      <c r="B115">
+        <v>1.3432299999999998E-5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116">
+        <v>58.4054</v>
+      </c>
+      <c r="B116">
+        <v>9.8620699999999996E-6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117">
+        <v>58.88</v>
+      </c>
+      <c r="B117">
+        <v>1.8895099999999998E-5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118">
+        <v>59.331600000000002</v>
+      </c>
+      <c r="B118">
+        <v>1.0890599999999999E-5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119">
         <v>60</v>
       </c>
-      <c r="B15" s="1">
-        <v>14201900</v>
+      <c r="B119">
+        <v>9.9612399999999987E-8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120">
+        <v>60</v>
+      </c>
+      <c r="B120">
+        <v>7.2996499999999988E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>